<commit_message>
Tidying up sailing folder. Annotating AllTCFs_2013-14.xlsx
</commit_message>
<xml_diff>
--- a/AllTCFs_2013-14.xlsx
+++ b/AllTCFs_2013-14.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="33555" windowHeight="19725"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="33555" windowHeight="19725" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="AllTCFs" sheetId="1" r:id="rId1"/>
+    <sheet name="Notes" sheetId="2" r:id="rId1"/>
+    <sheet name="AllTCFs_2013-14" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">AllTCFs!$B$1:$AB$1271</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'AllTCFs_2013-14'!$B$1:$AB$1271</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7175" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7233" uniqueCount="184">
   <si>
     <t>Date</t>
   </si>
@@ -488,6 +489,87 @@
   </si>
   <si>
     <t>Wai Aniwa</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Handicap type</t>
+  </si>
+  <si>
+    <t>Series name</t>
+  </si>
+  <si>
+    <t>Race number</t>
+  </si>
+  <si>
+    <t>Division</t>
+  </si>
+  <si>
+    <t>1 denotes TCF manually reset by handicapper; 0 otherwise</t>
+  </si>
+  <si>
+    <t>Algorithm used to update TCF - 1 = 'Method E' used in 2013-14; 2 = unweighted average of 5 performances used in 2014-15</t>
+  </si>
+  <si>
+    <t>1 denotes scored by club handicap or all handicaps; 2 denotes scored on PHRF only</t>
+  </si>
+  <si>
+    <t>Elapsed time in seconds</t>
+  </si>
+  <si>
+    <t>Corrected (on club handicap) time in seconds</t>
+  </si>
+  <si>
+    <t>Reference time</t>
+  </si>
+  <si>
+    <t>Rank or place on club handicap applied by race scorer on the day</t>
+  </si>
+  <si>
+    <t>Actual rank or place on club handicap</t>
+  </si>
+  <si>
+    <t>Difference between the above two numbers</t>
+  </si>
+  <si>
+    <t>Rank or place on PHRF</t>
+  </si>
+  <si>
+    <t>Rank or place on IRC</t>
+  </si>
+  <si>
+    <t>IRC value</t>
+  </si>
+  <si>
+    <t>PHRF value</t>
+  </si>
+  <si>
+    <t>The club TCF (time correction factor) applied by the race scorer on the day</t>
+  </si>
+  <si>
+    <t>What the TCF actually should have been</t>
+  </si>
+  <si>
+    <t>The sailed-to TCF - a performance measure</t>
+  </si>
+  <si>
+    <t>Percentage difference between TCFactual and TCFst</t>
+  </si>
+  <si>
+    <t>TCFst clamped to change by no more or less than 3% from TCFactual - the value that feeds into the TCF update formula</t>
+  </si>
+  <si>
+    <t>Updated TCF to be used in the next race</t>
+  </si>
+  <si>
+    <t>See also https://github.com/drphilbishop/RPNYC_race_analysis.</t>
+  </si>
+  <si>
+    <t>Contact: Phil Bishop (drphil.bishop@gmail.com), RPNYC handicapper for 2013-14 season.</t>
   </si>
 </sst>
 </file>
@@ -975,7 +1057,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1002,6 +1084,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1344,13 +1428,265 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="118.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>183</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB1271"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1476,7 +1812,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3">
-        <v>41910</v>
+        <v>41545</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>27</v>
@@ -1556,7 +1892,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3">
-        <v>41910</v>
+        <v>41545</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>27</v>
@@ -1639,7 +1975,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3">
-        <v>41910</v>
+        <v>41545</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>27</v>
@@ -1722,7 +2058,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3">
-        <v>41910</v>
+        <v>41545</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>27</v>
@@ -1802,7 +2138,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3">
-        <v>41910</v>
+        <v>41545</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>27</v>
@@ -1882,7 +2218,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3">
-        <v>41910</v>
+        <v>41545</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>27</v>
@@ -1956,7 +2292,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3">
-        <v>41910</v>
+        <v>41545</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>27</v>
@@ -2036,7 +2372,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3">
-        <v>41910</v>
+        <v>41545</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>27</v>
@@ -2116,7 +2452,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3">
-        <v>41910</v>
+        <v>41545</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>27</v>
@@ -2199,7 +2535,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="3">
-        <v>41910</v>
+        <v>41545</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>27</v>
@@ -2234,7 +2570,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="3">
-        <v>41910</v>
+        <v>41545</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>27</v>
@@ -2308,7 +2644,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="3">
-        <v>41910</v>
+        <v>41545</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>27</v>
@@ -2388,7 +2724,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="3">
-        <v>41910</v>
+        <v>41545</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>27</v>
@@ -2468,7 +2804,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>27</v>
@@ -2542,7 +2878,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>27</v>
@@ -2622,7 +2958,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>27</v>
@@ -2705,7 +3041,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>27</v>
@@ -2788,7 +3124,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>27</v>
@@ -2868,7 +3204,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>27</v>
@@ -2948,7 +3284,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>27</v>
@@ -3028,7 +3364,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>27</v>
@@ -3108,7 +3444,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>27</v>
@@ -3188,7 +3524,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>27</v>
@@ -3271,7 +3607,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>27</v>
@@ -3351,7 +3687,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>27</v>
@@ -3434,7 +3770,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>27</v>
@@ -3508,7 +3844,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>27</v>
@@ -3588,7 +3924,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>27</v>
@@ -3668,7 +4004,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>27</v>
@@ -3742,7 +4078,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>27</v>
@@ -3825,7 +4161,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>27</v>
@@ -3905,7 +4241,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>27</v>
@@ -3985,7 +4321,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>27</v>
@@ -4065,7 +4401,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>27</v>
@@ -4145,7 +4481,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>27</v>
@@ -4180,7 +4516,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>27</v>
@@ -4260,7 +4596,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>27</v>
@@ -4340,7 +4676,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>27</v>
@@ -4420,7 +4756,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>27</v>
@@ -4494,7 +4830,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>27</v>
@@ -4574,7 +4910,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>27</v>
@@ -4657,7 +4993,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>27</v>
@@ -4737,7 +5073,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>27</v>
@@ -4817,7 +5153,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>27</v>
@@ -4897,7 +5233,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>27</v>
@@ -4977,7 +5313,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>27</v>
@@ -5060,7 +5396,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>27</v>
@@ -5140,7 +5476,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>27</v>
@@ -5214,7 +5550,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>27</v>
@@ -5294,7 +5630,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>27</v>
@@ -5377,7 +5713,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>27</v>
@@ -5457,7 +5793,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>27</v>
@@ -5540,7 +5876,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>27</v>
@@ -5620,7 +5956,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>27</v>
@@ -5700,7 +6036,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>27</v>
@@ -5780,7 +6116,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>27</v>
@@ -5863,7 +6199,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>27</v>
@@ -5943,7 +6279,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>27</v>
@@ -6023,7 +6359,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>64</v>
@@ -6097,7 +6433,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>64</v>
@@ -6171,7 +6507,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="3">
-        <v>41917</v>
+        <v>41552</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>64</v>
@@ -6245,7 +6581,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="3">
-        <v>41924</v>
+        <v>41559</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>27</v>
@@ -6319,7 +6655,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="3">
-        <v>41924</v>
+        <v>41559</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>27</v>
@@ -6399,7 +6735,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="3">
-        <v>41924</v>
+        <v>41559</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>27</v>
@@ -6479,7 +6815,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="3">
-        <v>41924</v>
+        <v>41559</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>27</v>
@@ -6553,7 +6889,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="3">
-        <v>41924</v>
+        <v>41559</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>27</v>
@@ -6633,7 +6969,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="3">
-        <v>41924</v>
+        <v>41559</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>27</v>
@@ -6713,7 +7049,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="3">
-        <v>41924</v>
+        <v>41559</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>27</v>
@@ -6793,7 +7129,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="3">
-        <v>41924</v>
+        <v>41559</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>27</v>
@@ -6867,7 +7203,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="3">
-        <v>41924</v>
+        <v>41559</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>27</v>
@@ -6941,7 +7277,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="3">
-        <v>41924</v>
+        <v>41559</v>
       </c>
       <c r="C72" s="4" t="s">
         <v>27</v>
@@ -7021,7 +7357,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="3">
-        <v>41924</v>
+        <v>41559</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>27</v>
@@ -7104,7 +7440,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="3">
-        <v>41924</v>
+        <v>41559</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>27</v>
@@ -7187,7 +7523,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="3">
-        <v>41924</v>
+        <v>41559</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>27</v>
@@ -7267,7 +7603,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="3">
-        <v>41924</v>
+        <v>41559</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>27</v>
@@ -7347,7 +7683,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="3">
-        <v>41924</v>
+        <v>41559</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>27</v>
@@ -7427,7 +7763,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="3">
-        <v>41924</v>
+        <v>41559</v>
       </c>
       <c r="C78" s="4" t="s">
         <v>27</v>
@@ -7507,7 +7843,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="3">
-        <v>41924</v>
+        <v>41559</v>
       </c>
       <c r="C79" s="4" t="s">
         <v>27</v>
@@ -7587,7 +7923,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="3">
-        <v>41924</v>
+        <v>41559</v>
       </c>
       <c r="C80" s="4" t="s">
         <v>27</v>
@@ -7667,7 +8003,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="3">
-        <v>41924</v>
+        <v>41559</v>
       </c>
       <c r="C81" s="4" t="s">
         <v>27</v>
@@ -7750,7 +8086,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="3">
-        <v>41924</v>
+        <v>41559</v>
       </c>
       <c r="C82" s="4" t="s">
         <v>27</v>
@@ -7830,7 +8166,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="3">
-        <v>41924</v>
+        <v>41559</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>27</v>
@@ -7910,7 +8246,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="3">
-        <v>41924</v>
+        <v>41559</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>27</v>
@@ -7993,7 +8329,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="3">
-        <v>41924</v>
+        <v>41559</v>
       </c>
       <c r="C85" s="4" t="s">
         <v>27</v>
@@ -8073,7 +8409,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="3">
-        <v>41924</v>
+        <v>41559</v>
       </c>
       <c r="C86" s="4" t="s">
         <v>27</v>
@@ -8147,7 +8483,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="3">
-        <v>41924</v>
+        <v>41559</v>
       </c>
       <c r="C87" s="4" t="s">
         <v>27</v>
@@ -8230,7 +8566,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="3">
-        <v>41924</v>
+        <v>41559</v>
       </c>
       <c r="C88" s="4" t="s">
         <v>27</v>
@@ -8310,7 +8646,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="3">
-        <v>41924</v>
+        <v>41559</v>
       </c>
       <c r="C89" s="4" t="s">
         <v>27</v>
@@ -8390,7 +8726,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="3">
-        <v>41924</v>
+        <v>41559</v>
       </c>
       <c r="C90" s="4" t="s">
         <v>27</v>
@@ -8470,7 +8806,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="3">
-        <v>41924</v>
+        <v>41559</v>
       </c>
       <c r="C91" s="4" t="s">
         <v>27</v>
@@ -8550,7 +8886,7 @@
         <v>91</v>
       </c>
       <c r="B92" s="3">
-        <v>41931</v>
+        <v>41566</v>
       </c>
       <c r="C92" s="4" t="s">
         <v>74</v>
@@ -8624,7 +8960,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="3">
-        <v>41931</v>
+        <v>41566</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>74</v>
@@ -8704,7 +9040,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="3">
-        <v>41931</v>
+        <v>41566</v>
       </c>
       <c r="C94" s="4" t="s">
         <v>74</v>
@@ -8787,7 +9123,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="3">
-        <v>41931</v>
+        <v>41566</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>74</v>
@@ -8867,7 +9203,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="3">
-        <v>41931</v>
+        <v>41566</v>
       </c>
       <c r="C96" s="4" t="s">
         <v>74</v>
@@ -8947,7 +9283,7 @@
         <v>96</v>
       </c>
       <c r="B97" s="3">
-        <v>41931</v>
+        <v>41566</v>
       </c>
       <c r="C97" s="4" t="s">
         <v>74</v>
@@ -9027,7 +9363,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="3">
-        <v>41931</v>
+        <v>41566</v>
       </c>
       <c r="C98" s="4" t="s">
         <v>74</v>
@@ -9107,7 +9443,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="3">
-        <v>41931</v>
+        <v>41566</v>
       </c>
       <c r="C99" s="4" t="s">
         <v>74</v>
@@ -9190,7 +9526,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="3">
-        <v>41931</v>
+        <v>41566</v>
       </c>
       <c r="C100" s="4" t="s">
         <v>74</v>
@@ -9270,7 +9606,7 @@
         <v>100</v>
       </c>
       <c r="B101" s="3">
-        <v>41931</v>
+        <v>41566</v>
       </c>
       <c r="C101" s="4" t="s">
         <v>74</v>
@@ -9350,7 +9686,7 @@
         <v>101</v>
       </c>
       <c r="B102" s="3">
-        <v>41944</v>
+        <v>41579</v>
       </c>
       <c r="C102" s="4" t="s">
         <v>76</v>
@@ -9385,7 +9721,7 @@
         <v>102</v>
       </c>
       <c r="B103" s="3">
-        <v>41944</v>
+        <v>41579</v>
       </c>
       <c r="C103" s="4" t="s">
         <v>76</v>
@@ -9420,7 +9756,7 @@
         <v>103</v>
       </c>
       <c r="B104" s="3">
-        <v>41944</v>
+        <v>41579</v>
       </c>
       <c r="C104" s="4" t="s">
         <v>76</v>
@@ -9455,7 +9791,7 @@
         <v>104</v>
       </c>
       <c r="B105" s="3">
-        <v>41944</v>
+        <v>41579</v>
       </c>
       <c r="C105" s="4" t="s">
         <v>76</v>
@@ -9490,7 +9826,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="3">
-        <v>41944</v>
+        <v>41579</v>
       </c>
       <c r="C106" s="4" t="s">
         <v>76</v>
@@ -9525,7 +9861,7 @@
         <v>106</v>
       </c>
       <c r="B107" s="3">
-        <v>41944</v>
+        <v>41579</v>
       </c>
       <c r="C107" s="4" t="s">
         <v>76</v>
@@ -9599,7 +9935,7 @@
         <v>107</v>
       </c>
       <c r="B108" s="3">
-        <v>41944</v>
+        <v>41579</v>
       </c>
       <c r="C108" s="4" t="s">
         <v>76</v>
@@ -9673,7 +10009,7 @@
         <v>108</v>
       </c>
       <c r="B109" s="3">
-        <v>41944</v>
+        <v>41579</v>
       </c>
       <c r="C109" s="4" t="s">
         <v>76</v>
@@ -9747,7 +10083,7 @@
         <v>109</v>
       </c>
       <c r="B110" s="3">
-        <v>41944</v>
+        <v>41579</v>
       </c>
       <c r="C110" s="4" t="s">
         <v>76</v>
@@ -9821,7 +10157,7 @@
         <v>110</v>
       </c>
       <c r="B111" s="3">
-        <v>41944</v>
+        <v>41579</v>
       </c>
       <c r="C111" s="4" t="s">
         <v>76</v>
@@ -9895,7 +10231,7 @@
         <v>111</v>
       </c>
       <c r="B112" s="3">
-        <v>41944</v>
+        <v>41579</v>
       </c>
       <c r="C112" s="4" t="s">
         <v>76</v>
@@ -9969,7 +10305,7 @@
         <v>112</v>
       </c>
       <c r="B113" s="3">
-        <v>41944</v>
+        <v>41579</v>
       </c>
       <c r="C113" s="4" t="s">
         <v>76</v>
@@ -10043,7 +10379,7 @@
         <v>113</v>
       </c>
       <c r="B114" s="3">
-        <v>41944</v>
+        <v>41579</v>
       </c>
       <c r="C114" s="4" t="s">
         <v>76</v>
@@ -10117,7 +10453,7 @@
         <v>114</v>
       </c>
       <c r="B115" s="3">
-        <v>41944</v>
+        <v>41579</v>
       </c>
       <c r="C115" s="4" t="s">
         <v>76</v>
@@ -10191,7 +10527,7 @@
         <v>115</v>
       </c>
       <c r="B116" s="3">
-        <v>41944</v>
+        <v>41579</v>
       </c>
       <c r="C116" s="4" t="s">
         <v>76</v>
@@ -10265,7 +10601,7 @@
         <v>116</v>
       </c>
       <c r="B117" s="3">
-        <v>41944</v>
+        <v>41579</v>
       </c>
       <c r="C117" s="4" t="s">
         <v>76</v>
@@ -10339,7 +10675,7 @@
         <v>117</v>
       </c>
       <c r="B118" s="3">
-        <v>41944</v>
+        <v>41579</v>
       </c>
       <c r="C118" s="4" t="s">
         <v>76</v>
@@ -10413,7 +10749,7 @@
         <v>118</v>
       </c>
       <c r="B119" s="3">
-        <v>41944</v>
+        <v>41579</v>
       </c>
       <c r="C119" s="4" t="s">
         <v>76</v>
@@ -10487,7 +10823,7 @@
         <v>119</v>
       </c>
       <c r="B120" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C120" s="4" t="s">
         <v>27</v>
@@ -10567,7 +10903,7 @@
         <v>120</v>
       </c>
       <c r="B121" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C121" s="4" t="s">
         <v>27</v>
@@ -10647,7 +10983,7 @@
         <v>121</v>
       </c>
       <c r="B122" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C122" s="4" t="s">
         <v>27</v>
@@ -10727,7 +11063,7 @@
         <v>122</v>
       </c>
       <c r="B123" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C123" s="4" t="s">
         <v>27</v>
@@ -10807,7 +11143,7 @@
         <v>123</v>
       </c>
       <c r="B124" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C124" s="4" t="s">
         <v>27</v>
@@ -10890,7 +11226,7 @@
         <v>124</v>
       </c>
       <c r="B125" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C125" s="4" t="s">
         <v>27</v>
@@ -10973,7 +11309,7 @@
         <v>125</v>
       </c>
       <c r="B126" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C126" s="4" t="s">
         <v>27</v>
@@ -11053,7 +11389,7 @@
         <v>126</v>
       </c>
       <c r="B127" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C127" s="4" t="s">
         <v>27</v>
@@ -11133,7 +11469,7 @@
         <v>127</v>
       </c>
       <c r="B128" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C128" s="4" t="s">
         <v>27</v>
@@ -11213,7 +11549,7 @@
         <v>128</v>
       </c>
       <c r="B129" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C129" s="4" t="s">
         <v>27</v>
@@ -11287,7 +11623,7 @@
         <v>129</v>
       </c>
       <c r="B130" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C130" s="4" t="s">
         <v>27</v>
@@ -11367,7 +11703,7 @@
         <v>130</v>
       </c>
       <c r="B131" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C131" s="4" t="s">
         <v>27</v>
@@ -11450,7 +11786,7 @@
         <v>131</v>
       </c>
       <c r="B132" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C132" s="4" t="s">
         <v>27</v>
@@ -11533,7 +11869,7 @@
         <v>132</v>
       </c>
       <c r="B133" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C133" s="4" t="s">
         <v>27</v>
@@ -11616,7 +11952,7 @@
         <v>133</v>
       </c>
       <c r="B134" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C134" s="4" t="s">
         <v>27</v>
@@ -11696,7 +12032,7 @@
         <v>134</v>
       </c>
       <c r="B135" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C135" s="4" t="s">
         <v>27</v>
@@ -11770,7 +12106,7 @@
         <v>135</v>
       </c>
       <c r="B136" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C136" s="4" t="s">
         <v>27</v>
@@ -11850,7 +12186,7 @@
         <v>136</v>
       </c>
       <c r="B137" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C137" s="4" t="s">
         <v>27</v>
@@ -11933,7 +12269,7 @@
         <v>137</v>
       </c>
       <c r="B138" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C138" s="4" t="s">
         <v>27</v>
@@ -12013,7 +12349,7 @@
         <v>138</v>
       </c>
       <c r="B139" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C139" s="4" t="s">
         <v>27</v>
@@ -12048,7 +12384,7 @@
         <v>139</v>
       </c>
       <c r="B140" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C140" s="4" t="s">
         <v>27</v>
@@ -12122,7 +12458,7 @@
         <v>140</v>
       </c>
       <c r="B141" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C141" s="4" t="s">
         <v>27</v>
@@ -12196,7 +12532,7 @@
         <v>141</v>
       </c>
       <c r="B142" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C142" s="4" t="s">
         <v>27</v>
@@ -12276,7 +12612,7 @@
         <v>142</v>
       </c>
       <c r="B143" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C143" s="4" t="s">
         <v>27</v>
@@ -12350,7 +12686,7 @@
         <v>143</v>
       </c>
       <c r="B144" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C144" s="4" t="s">
         <v>27</v>
@@ -12430,7 +12766,7 @@
         <v>144</v>
       </c>
       <c r="B145" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C145" s="4" t="s">
         <v>27</v>
@@ -12510,7 +12846,7 @@
         <v>145</v>
       </c>
       <c r="B146" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C146" s="4" t="s">
         <v>27</v>
@@ -12584,7 +12920,7 @@
         <v>146</v>
       </c>
       <c r="B147" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C147" s="4" t="s">
         <v>64</v>
@@ -12619,7 +12955,7 @@
         <v>147</v>
       </c>
       <c r="B148" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C148" s="4" t="s">
         <v>64</v>
@@ -12693,7 +13029,7 @@
         <v>148</v>
       </c>
       <c r="B149" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C149" s="4" t="s">
         <v>82</v>
@@ -12728,7 +13064,7 @@
         <v>149</v>
       </c>
       <c r="B150" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C150" s="4" t="s">
         <v>82</v>
@@ -12808,7 +13144,7 @@
         <v>150</v>
       </c>
       <c r="B151" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C151" s="4" t="s">
         <v>82</v>
@@ -12888,7 +13224,7 @@
         <v>151</v>
       </c>
       <c r="B152" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C152" s="4" t="s">
         <v>82</v>
@@ -12968,7 +13304,7 @@
         <v>152</v>
       </c>
       <c r="B153" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C153" s="4" t="s">
         <v>82</v>
@@ -13042,7 +13378,7 @@
         <v>153</v>
       </c>
       <c r="B154" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C154" s="4" t="s">
         <v>82</v>
@@ -13125,7 +13461,7 @@
         <v>154</v>
       </c>
       <c r="B155" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C155" s="4" t="s">
         <v>82</v>
@@ -13199,7 +13535,7 @@
         <v>155</v>
       </c>
       <c r="B156" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C156" s="4" t="s">
         <v>82</v>
@@ -13279,7 +13615,7 @@
         <v>156</v>
       </c>
       <c r="B157" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C157" s="4" t="s">
         <v>82</v>
@@ -13359,7 +13695,7 @@
         <v>157</v>
       </c>
       <c r="B158" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C158" s="4" t="s">
         <v>82</v>
@@ -13442,7 +13778,7 @@
         <v>158</v>
       </c>
       <c r="B159" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C159" s="4" t="s">
         <v>82</v>
@@ -13522,7 +13858,7 @@
         <v>159</v>
       </c>
       <c r="B160" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C160" s="4" t="s">
         <v>82</v>
@@ -13596,7 +13932,7 @@
         <v>160</v>
       </c>
       <c r="B161" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C161" s="4" t="s">
         <v>82</v>
@@ -13676,7 +14012,7 @@
         <v>161</v>
       </c>
       <c r="B162" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C162" s="4" t="s">
         <v>82</v>
@@ -13759,7 +14095,7 @@
         <v>162</v>
       </c>
       <c r="B163" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C163" s="4" t="s">
         <v>82</v>
@@ -13833,7 +14169,7 @@
         <v>163</v>
       </c>
       <c r="B164" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C164" s="4" t="s">
         <v>82</v>
@@ -13907,7 +14243,7 @@
         <v>164</v>
       </c>
       <c r="B165" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C165" s="4" t="s">
         <v>82</v>
@@ -13990,7 +14326,7 @@
         <v>165</v>
       </c>
       <c r="B166" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C166" s="4" t="s">
         <v>82</v>
@@ -14073,7 +14409,7 @@
         <v>166</v>
       </c>
       <c r="B167" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C167" s="4" t="s">
         <v>82</v>
@@ -14156,7 +14492,7 @@
         <v>167</v>
       </c>
       <c r="B168" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C168" s="4" t="s">
         <v>82</v>
@@ -14236,7 +14572,7 @@
         <v>168</v>
       </c>
       <c r="B169" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C169" s="4" t="s">
         <v>82</v>
@@ -14316,7 +14652,7 @@
         <v>169</v>
       </c>
       <c r="B170" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C170" s="4" t="s">
         <v>82</v>
@@ -14396,7 +14732,7 @@
         <v>170</v>
       </c>
       <c r="B171" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C171" s="4" t="s">
         <v>82</v>
@@ -14476,7 +14812,7 @@
         <v>171</v>
       </c>
       <c r="B172" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C172" s="4" t="s">
         <v>82</v>
@@ -14556,7 +14892,7 @@
         <v>172</v>
       </c>
       <c r="B173" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C173" s="4" t="s">
         <v>82</v>
@@ -14636,7 +14972,7 @@
         <v>173</v>
       </c>
       <c r="B174" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C174" s="4" t="s">
         <v>82</v>
@@ -14716,7 +15052,7 @@
         <v>174</v>
       </c>
       <c r="B175" s="3">
-        <v>41945</v>
+        <v>41580</v>
       </c>
       <c r="C175" s="4" t="s">
         <v>82</v>
@@ -14790,7 +15126,7 @@
         <v>175</v>
       </c>
       <c r="B176" s="3">
-        <v>41949</v>
+        <v>41584</v>
       </c>
       <c r="C176" s="4" t="s">
         <v>85</v>
@@ -14870,7 +15206,7 @@
         <v>176</v>
       </c>
       <c r="B177" s="3">
-        <v>41949</v>
+        <v>41584</v>
       </c>
       <c r="C177" s="4" t="s">
         <v>85</v>
@@ -14950,7 +15286,7 @@
         <v>177</v>
       </c>
       <c r="B178" s="3">
-        <v>41951</v>
+        <v>41586</v>
       </c>
       <c r="C178" s="4" t="s">
         <v>76</v>
@@ -15024,7 +15360,7 @@
         <v>178</v>
       </c>
       <c r="B179" s="3">
-        <v>41951</v>
+        <v>41586</v>
       </c>
       <c r="C179" s="4" t="s">
         <v>76</v>
@@ -15098,7 +15434,7 @@
         <v>179</v>
       </c>
       <c r="B180" s="3">
-        <v>41951</v>
+        <v>41586</v>
       </c>
       <c r="C180" s="4" t="s">
         <v>76</v>
@@ -15172,7 +15508,7 @@
         <v>180</v>
       </c>
       <c r="B181" s="3">
-        <v>41951</v>
+        <v>41586</v>
       </c>
       <c r="C181" s="4" t="s">
         <v>76</v>
@@ -15246,7 +15582,7 @@
         <v>181</v>
       </c>
       <c r="B182" s="3">
-        <v>41951</v>
+        <v>41586</v>
       </c>
       <c r="C182" s="4" t="s">
         <v>76</v>
@@ -15320,7 +15656,7 @@
         <v>182</v>
       </c>
       <c r="B183" s="3">
-        <v>41951</v>
+        <v>41586</v>
       </c>
       <c r="C183" s="4" t="s">
         <v>76</v>
@@ -15394,7 +15730,7 @@
         <v>183</v>
       </c>
       <c r="B184" s="3">
-        <v>41951</v>
+        <v>41586</v>
       </c>
       <c r="C184" s="4" t="s">
         <v>76</v>
@@ -15468,7 +15804,7 @@
         <v>184</v>
       </c>
       <c r="B185" s="3">
-        <v>41952</v>
+        <v>41587</v>
       </c>
       <c r="C185" s="4" t="s">
         <v>85</v>
@@ -15542,7 +15878,7 @@
         <v>185</v>
       </c>
       <c r="B186" s="3">
-        <v>41952</v>
+        <v>41587</v>
       </c>
       <c r="C186" s="4" t="s">
         <v>85</v>
@@ -15622,7 +15958,7 @@
         <v>186</v>
       </c>
       <c r="B187" s="3">
-        <v>41952</v>
+        <v>41587</v>
       </c>
       <c r="C187" s="4" t="s">
         <v>85</v>
@@ -15702,7 +16038,7 @@
         <v>187</v>
       </c>
       <c r="B188" s="3">
-        <v>41952</v>
+        <v>41587</v>
       </c>
       <c r="C188" s="4" t="s">
         <v>85</v>
@@ -15776,7 +16112,7 @@
         <v>188</v>
       </c>
       <c r="B189" s="3">
-        <v>41952</v>
+        <v>41587</v>
       </c>
       <c r="C189" s="4" t="s">
         <v>85</v>
@@ -15856,7 +16192,7 @@
         <v>189</v>
       </c>
       <c r="B190" s="3">
-        <v>41952</v>
+        <v>41587</v>
       </c>
       <c r="C190" s="4" t="s">
         <v>85</v>
@@ -15936,7 +16272,7 @@
         <v>190</v>
       </c>
       <c r="B191" s="3">
-        <v>41952</v>
+        <v>41587</v>
       </c>
       <c r="C191" s="4" t="s">
         <v>85</v>
@@ -16016,7 +16352,7 @@
         <v>191</v>
       </c>
       <c r="B192" s="3">
-        <v>41952</v>
+        <v>41587</v>
       </c>
       <c r="C192" s="4" t="s">
         <v>85</v>
@@ -16090,7 +16426,7 @@
         <v>192</v>
       </c>
       <c r="B193" s="3">
-        <v>41952</v>
+        <v>41587</v>
       </c>
       <c r="C193" s="4" t="s">
         <v>85</v>
@@ -16170,7 +16506,7 @@
         <v>193</v>
       </c>
       <c r="B194" s="3">
-        <v>41952</v>
+        <v>41587</v>
       </c>
       <c r="C194" s="4" t="s">
         <v>85</v>
@@ -16244,7 +16580,7 @@
         <v>194</v>
       </c>
       <c r="B195" s="3">
-        <v>41952</v>
+        <v>41587</v>
       </c>
       <c r="C195" s="4" t="s">
         <v>90</v>
@@ -16324,7 +16660,7 @@
         <v>195</v>
       </c>
       <c r="B196" s="3">
-        <v>41952</v>
+        <v>41587</v>
       </c>
       <c r="C196" s="4" t="s">
         <v>90</v>
@@ -16407,7 +16743,7 @@
         <v>196</v>
       </c>
       <c r="B197" s="3">
-        <v>41952</v>
+        <v>41587</v>
       </c>
       <c r="C197" s="4" t="s">
         <v>90</v>
@@ -16490,7 +16826,7 @@
         <v>197</v>
       </c>
       <c r="B198" s="3">
-        <v>41952</v>
+        <v>41587</v>
       </c>
       <c r="C198" s="4" t="s">
         <v>90</v>
@@ -16564,7 +16900,7 @@
         <v>198</v>
       </c>
       <c r="B199" s="3">
-        <v>41952</v>
+        <v>41587</v>
       </c>
       <c r="C199" s="4" t="s">
         <v>90</v>
@@ -16647,7 +16983,7 @@
         <v>199</v>
       </c>
       <c r="B200" s="3">
-        <v>41952</v>
+        <v>41587</v>
       </c>
       <c r="C200" s="4" t="s">
         <v>90</v>
@@ -16727,7 +17063,7 @@
         <v>200</v>
       </c>
       <c r="B201" s="3">
-        <v>41952</v>
+        <v>41587</v>
       </c>
       <c r="C201" s="4" t="s">
         <v>90</v>
@@ -16801,7 +17137,7 @@
         <v>201</v>
       </c>
       <c r="B202" s="3">
-        <v>41952</v>
+        <v>41587</v>
       </c>
       <c r="C202" s="4" t="s">
         <v>90</v>
@@ -16884,7 +17220,7 @@
         <v>202</v>
       </c>
       <c r="B203" s="3">
-        <v>41952</v>
+        <v>41587</v>
       </c>
       <c r="C203" s="4" t="s">
         <v>90</v>
@@ -16967,7 +17303,7 @@
         <v>203</v>
       </c>
       <c r="B204" s="3">
-        <v>41952</v>
+        <v>41587</v>
       </c>
       <c r="C204" s="4" t="s">
         <v>90</v>
@@ -17047,7 +17383,7 @@
         <v>204</v>
       </c>
       <c r="B205" s="3">
-        <v>41952</v>
+        <v>41587</v>
       </c>
       <c r="C205" s="4" t="s">
         <v>90</v>
@@ -17127,7 +17463,7 @@
         <v>205</v>
       </c>
       <c r="B206" s="3">
-        <v>41952</v>
+        <v>41587</v>
       </c>
       <c r="C206" s="4" t="s">
         <v>90</v>
@@ -17207,7 +17543,7 @@
         <v>206</v>
       </c>
       <c r="B207" s="3">
-        <v>41952</v>
+        <v>41587</v>
       </c>
       <c r="C207" s="4" t="s">
         <v>90</v>
@@ -17287,7 +17623,7 @@
         <v>207</v>
       </c>
       <c r="B208" s="3">
-        <v>41956</v>
+        <v>41591</v>
       </c>
       <c r="C208" s="4" t="s">
         <v>85</v>
@@ -17370,7 +17706,7 @@
         <v>208</v>
       </c>
       <c r="B209" s="3">
-        <v>41956</v>
+        <v>41591</v>
       </c>
       <c r="C209" s="4" t="s">
         <v>85</v>
@@ -17453,7 +17789,7 @@
         <v>209</v>
       </c>
       <c r="B210" s="3">
-        <v>41956</v>
+        <v>41591</v>
       </c>
       <c r="C210" s="4" t="s">
         <v>85</v>
@@ -17533,7 +17869,7 @@
         <v>210</v>
       </c>
       <c r="B211" s="3">
-        <v>41956</v>
+        <v>41591</v>
       </c>
       <c r="C211" s="4" t="s">
         <v>85</v>
@@ -17613,7 +17949,7 @@
         <v>211</v>
       </c>
       <c r="B212" s="3">
-        <v>41956</v>
+        <v>41591</v>
       </c>
       <c r="C212" s="4" t="s">
         <v>85</v>
@@ -17687,7 +18023,7 @@
         <v>212</v>
       </c>
       <c r="B213" s="3">
-        <v>41956</v>
+        <v>41591</v>
       </c>
       <c r="C213" s="4" t="s">
         <v>85</v>
@@ -17767,7 +18103,7 @@
         <v>213</v>
       </c>
       <c r="B214" s="3">
-        <v>41956</v>
+        <v>41591</v>
       </c>
       <c r="C214" s="4" t="s">
         <v>85</v>
@@ -17850,7 +18186,7 @@
         <v>214</v>
       </c>
       <c r="B215" s="3">
-        <v>41958</v>
+        <v>41593</v>
       </c>
       <c r="C215" s="4" t="s">
         <v>76</v>
@@ -17924,7 +18260,7 @@
         <v>215</v>
       </c>
       <c r="B216" s="3">
-        <v>41958</v>
+        <v>41593</v>
       </c>
       <c r="C216" s="4" t="s">
         <v>76</v>
@@ -17998,7 +18334,7 @@
         <v>216</v>
       </c>
       <c r="B217" s="3">
-        <v>41958</v>
+        <v>41593</v>
       </c>
       <c r="C217" s="4" t="s">
         <v>76</v>
@@ -18072,7 +18408,7 @@
         <v>217</v>
       </c>
       <c r="B218" s="3">
-        <v>41958</v>
+        <v>41593</v>
       </c>
       <c r="C218" s="4" t="s">
         <v>76</v>
@@ -18146,7 +18482,7 @@
         <v>218</v>
       </c>
       <c r="B219" s="3">
-        <v>41958</v>
+        <v>41593</v>
       </c>
       <c r="C219" s="4" t="s">
         <v>76</v>
@@ -18220,7 +18556,7 @@
         <v>219</v>
       </c>
       <c r="B220" s="3">
-        <v>41958</v>
+        <v>41593</v>
       </c>
       <c r="C220" s="4" t="s">
         <v>76</v>
@@ -18294,7 +18630,7 @@
         <v>220</v>
       </c>
       <c r="B221" s="3">
-        <v>41958</v>
+        <v>41593</v>
       </c>
       <c r="C221" s="4" t="s">
         <v>76</v>
@@ -18368,7 +18704,7 @@
         <v>221</v>
       </c>
       <c r="B222" s="3">
-        <v>41959</v>
+        <v>41594</v>
       </c>
       <c r="C222" s="4" t="s">
         <v>27</v>
@@ -18403,7 +18739,7 @@
         <v>222</v>
       </c>
       <c r="B223" s="3">
-        <v>41959</v>
+        <v>41594</v>
       </c>
       <c r="C223" s="4" t="s">
         <v>27</v>
@@ -18438,7 +18774,7 @@
         <v>223</v>
       </c>
       <c r="B224" s="3">
-        <v>41959</v>
+        <v>41594</v>
       </c>
       <c r="C224" s="4" t="s">
         <v>27</v>
@@ -18518,7 +18854,7 @@
         <v>224</v>
       </c>
       <c r="B225" s="3">
-        <v>41959</v>
+        <v>41594</v>
       </c>
       <c r="C225" s="4" t="s">
         <v>27</v>
@@ -18601,7 +18937,7 @@
         <v>225</v>
       </c>
       <c r="B226" s="3">
-        <v>41959</v>
+        <v>41594</v>
       </c>
       <c r="C226" s="4" t="s">
         <v>27</v>
@@ -18681,7 +19017,7 @@
         <v>226</v>
       </c>
       <c r="B227" s="3">
-        <v>41959</v>
+        <v>41594</v>
       </c>
       <c r="C227" s="4" t="s">
         <v>27</v>
@@ -18761,7 +19097,7 @@
         <v>227</v>
       </c>
       <c r="B228" s="3">
-        <v>41959</v>
+        <v>41594</v>
       </c>
       <c r="C228" s="4" t="s">
         <v>27</v>
@@ -18844,7 +19180,7 @@
         <v>228</v>
       </c>
       <c r="B229" s="3">
-        <v>41959</v>
+        <v>41594</v>
       </c>
       <c r="C229" s="4" t="s">
         <v>27</v>
@@ -18924,7 +19260,7 @@
         <v>229</v>
       </c>
       <c r="B230" s="3">
-        <v>41959</v>
+        <v>41594</v>
       </c>
       <c r="C230" s="4" t="s">
         <v>27</v>
@@ -19004,7 +19340,7 @@
         <v>230</v>
       </c>
       <c r="B231" s="3">
-        <v>41959</v>
+        <v>41594</v>
       </c>
       <c r="C231" s="4" t="s">
         <v>27</v>
@@ -19084,7 +19420,7 @@
         <v>231</v>
       </c>
       <c r="B232" s="3">
-        <v>41959</v>
+        <v>41594</v>
       </c>
       <c r="C232" s="4" t="s">
         <v>27</v>
@@ -19164,7 +19500,7 @@
         <v>232</v>
       </c>
       <c r="B233" s="3">
-        <v>41959</v>
+        <v>41594</v>
       </c>
       <c r="C233" s="4" t="s">
         <v>27</v>
@@ -19247,7 +19583,7 @@
         <v>233</v>
       </c>
       <c r="B234" s="3">
-        <v>41959</v>
+        <v>41594</v>
       </c>
       <c r="C234" s="4" t="s">
         <v>27</v>
@@ -19327,7 +19663,7 @@
         <v>234</v>
       </c>
       <c r="B235" s="3">
-        <v>41959</v>
+        <v>41594</v>
       </c>
       <c r="C235" s="4" t="s">
         <v>27</v>
@@ -19401,7 +19737,7 @@
         <v>235</v>
       </c>
       <c r="B236" s="3">
-        <v>41959</v>
+        <v>41594</v>
       </c>
       <c r="C236" s="4" t="s">
         <v>27</v>
@@ -19481,7 +19817,7 @@
         <v>236</v>
       </c>
       <c r="B237" s="3">
-        <v>41959</v>
+        <v>41594</v>
       </c>
       <c r="C237" s="4" t="s">
         <v>27</v>
@@ -19516,7 +19852,7 @@
         <v>237</v>
       </c>
       <c r="B238" s="3">
-        <v>41959</v>
+        <v>41594</v>
       </c>
       <c r="C238" s="4" t="s">
         <v>27</v>
@@ -19596,7 +19932,7 @@
         <v>238</v>
       </c>
       <c r="B239" s="3">
-        <v>41959</v>
+        <v>41594</v>
       </c>
       <c r="C239" s="4" t="s">
         <v>27</v>
@@ -19676,7 +20012,7 @@
         <v>239</v>
       </c>
       <c r="B240" s="3">
-        <v>41959</v>
+        <v>41594</v>
       </c>
       <c r="C240" s="4" t="s">
         <v>27</v>
@@ -19756,7 +20092,7 @@
         <v>240</v>
       </c>
       <c r="B241" s="3">
-        <v>41959</v>
+        <v>41594</v>
       </c>
       <c r="C241" s="4" t="s">
         <v>27</v>
@@ -19836,7 +20172,7 @@
         <v>241</v>
       </c>
       <c r="B242" s="3">
-        <v>41959</v>
+        <v>41594</v>
       </c>
       <c r="C242" s="4" t="s">
         <v>27</v>
@@ -19916,7 +20252,7 @@
         <v>242</v>
       </c>
       <c r="B243" s="3">
-        <v>41959</v>
+        <v>41594</v>
       </c>
       <c r="C243" s="4" t="s">
         <v>27</v>
@@ -19996,7 +20332,7 @@
         <v>243</v>
       </c>
       <c r="B244" s="3">
-        <v>41959</v>
+        <v>41594</v>
       </c>
       <c r="C244" s="4" t="s">
         <v>27</v>
@@ -20070,7 +20406,7 @@
         <v>244</v>
       </c>
       <c r="B245" s="3">
-        <v>41963</v>
+        <v>41598</v>
       </c>
       <c r="C245" s="4" t="s">
         <v>85</v>
@@ -20150,7 +20486,7 @@
         <v>245</v>
       </c>
       <c r="B246" s="3">
-        <v>41963</v>
+        <v>41598</v>
       </c>
       <c r="C246" s="4" t="s">
         <v>85</v>
@@ -20233,7 +20569,7 @@
         <v>246</v>
       </c>
       <c r="B247" s="3">
-        <v>41963</v>
+        <v>41598</v>
       </c>
       <c r="C247" s="4" t="s">
         <v>85</v>
@@ -20313,7 +20649,7 @@
         <v>247</v>
       </c>
       <c r="B248" s="3">
-        <v>41963</v>
+        <v>41598</v>
       </c>
       <c r="C248" s="4" t="s">
         <v>85</v>
@@ -20387,7 +20723,7 @@
         <v>248</v>
       </c>
       <c r="B249" s="3">
-        <v>41963</v>
+        <v>41598</v>
       </c>
       <c r="C249" s="4" t="s">
         <v>85</v>
@@ -20467,7 +20803,7 @@
         <v>249</v>
       </c>
       <c r="B250" s="3">
-        <v>41963</v>
+        <v>41598</v>
       </c>
       <c r="C250" s="4" t="s">
         <v>85</v>
@@ -20547,7 +20883,7 @@
         <v>250</v>
       </c>
       <c r="B251" s="3">
-        <v>41963</v>
+        <v>41598</v>
       </c>
       <c r="C251" s="4" t="s">
         <v>85</v>
@@ -20630,7 +20966,7 @@
         <v>251</v>
       </c>
       <c r="B252" s="3">
-        <v>41963</v>
+        <v>41598</v>
       </c>
       <c r="C252" s="4" t="s">
         <v>85</v>
@@ -20710,7 +21046,7 @@
         <v>252</v>
       </c>
       <c r="B253" s="3">
-        <v>41963</v>
+        <v>41598</v>
       </c>
       <c r="C253" s="4" t="s">
         <v>85</v>
@@ -20784,7 +21120,7 @@
         <v>253</v>
       </c>
       <c r="B254" s="3">
-        <v>41963</v>
+        <v>41598</v>
       </c>
       <c r="C254" s="4" t="s">
         <v>85</v>
@@ -20864,7 +21200,7 @@
         <v>254</v>
       </c>
       <c r="B255" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C255" s="4" t="s">
         <v>27</v>
@@ -20944,7 +21280,7 @@
         <v>255</v>
       </c>
       <c r="B256" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C256" s="4" t="s">
         <v>27</v>
@@ -21024,7 +21360,7 @@
         <v>256</v>
       </c>
       <c r="B257" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C257" s="4" t="s">
         <v>27</v>
@@ -21104,7 +21440,7 @@
         <v>257</v>
       </c>
       <c r="B258" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C258" s="4" t="s">
         <v>27</v>
@@ -21187,7 +21523,7 @@
         <v>258</v>
       </c>
       <c r="B259" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C259" s="4" t="s">
         <v>27</v>
@@ -21267,7 +21603,7 @@
         <v>259</v>
       </c>
       <c r="B260" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C260" s="4" t="s">
         <v>27</v>
@@ -21347,7 +21683,7 @@
         <v>260</v>
       </c>
       <c r="B261" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C261" s="4" t="s">
         <v>27</v>
@@ -21427,7 +21763,7 @@
         <v>261</v>
       </c>
       <c r="B262" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C262" s="4" t="s">
         <v>27</v>
@@ -21510,7 +21846,7 @@
         <v>262</v>
       </c>
       <c r="B263" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C263" s="4" t="s">
         <v>27</v>
@@ -21590,7 +21926,7 @@
         <v>263</v>
       </c>
       <c r="B264" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C264" s="4" t="s">
         <v>27</v>
@@ -21670,7 +22006,7 @@
         <v>264</v>
       </c>
       <c r="B265" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C265" s="4" t="s">
         <v>27</v>
@@ -21753,7 +22089,7 @@
         <v>265</v>
       </c>
       <c r="B266" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C266" s="4" t="s">
         <v>27</v>
@@ -21836,7 +22172,7 @@
         <v>266</v>
       </c>
       <c r="B267" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C267" s="4" t="s">
         <v>27</v>
@@ -21916,7 +22252,7 @@
         <v>267</v>
       </c>
       <c r="B268" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C268" s="4" t="s">
         <v>27</v>
@@ -21990,7 +22326,7 @@
         <v>268</v>
       </c>
       <c r="B269" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C269" s="4" t="s">
         <v>27</v>
@@ -22073,7 +22409,7 @@
         <v>269</v>
       </c>
       <c r="B270" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C270" s="4" t="s">
         <v>27</v>
@@ -22147,7 +22483,7 @@
         <v>270</v>
       </c>
       <c r="B271" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C271" s="4" t="s">
         <v>27</v>
@@ -22227,7 +22563,7 @@
         <v>271</v>
       </c>
       <c r="B272" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C272" s="4" t="s">
         <v>27</v>
@@ -22307,7 +22643,7 @@
         <v>272</v>
       </c>
       <c r="B273" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C273" s="4" t="s">
         <v>27</v>
@@ -22387,7 +22723,7 @@
         <v>273</v>
       </c>
       <c r="B274" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C274" s="4" t="s">
         <v>27</v>
@@ -22461,7 +22797,7 @@
         <v>274</v>
       </c>
       <c r="B275" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C275" s="4" t="s">
         <v>27</v>
@@ -22544,7 +22880,7 @@
         <v>275</v>
       </c>
       <c r="B276" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C276" s="4" t="s">
         <v>27</v>
@@ -22618,7 +22954,7 @@
         <v>276</v>
       </c>
       <c r="B277" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C277" s="4" t="s">
         <v>27</v>
@@ -22698,7 +23034,7 @@
         <v>277</v>
       </c>
       <c r="B278" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C278" s="4" t="s">
         <v>27</v>
@@ -22778,7 +23114,7 @@
         <v>278</v>
       </c>
       <c r="B279" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C279" s="4" t="s">
         <v>27</v>
@@ -22858,7 +23194,7 @@
         <v>279</v>
       </c>
       <c r="B280" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C280" s="4" t="s">
         <v>27</v>
@@ -22938,7 +23274,7 @@
         <v>280</v>
       </c>
       <c r="B281" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C281" s="4" t="s">
         <v>27</v>
@@ -23012,7 +23348,7 @@
         <v>281</v>
       </c>
       <c r="B282" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C282" s="4" t="s">
         <v>27</v>
@@ -23086,7 +23422,7 @@
         <v>282</v>
       </c>
       <c r="B283" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C283" s="4" t="s">
         <v>27</v>
@@ -23166,7 +23502,7 @@
         <v>283</v>
       </c>
       <c r="B284" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C284" s="4" t="s">
         <v>27</v>
@@ -23246,7 +23582,7 @@
         <v>284</v>
       </c>
       <c r="B285" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C285" s="4" t="s">
         <v>27</v>
@@ -23326,7 +23662,7 @@
         <v>285</v>
       </c>
       <c r="B286" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C286" s="4" t="s">
         <v>27</v>
@@ -23409,7 +23745,7 @@
         <v>286</v>
       </c>
       <c r="B287" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C287" s="4" t="s">
         <v>27</v>
@@ -23489,7 +23825,7 @@
         <v>287</v>
       </c>
       <c r="B288" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C288" s="4" t="s">
         <v>27</v>
@@ -23569,7 +23905,7 @@
         <v>288</v>
       </c>
       <c r="B289" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C289" s="4" t="s">
         <v>27</v>
@@ -23649,7 +23985,7 @@
         <v>289</v>
       </c>
       <c r="B290" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C290" s="4" t="s">
         <v>27</v>
@@ -23729,7 +24065,7 @@
         <v>290</v>
       </c>
       <c r="B291" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C291" s="4" t="s">
         <v>27</v>
@@ -23809,7 +24145,7 @@
         <v>291</v>
       </c>
       <c r="B292" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C292" s="4" t="s">
         <v>27</v>
@@ -23889,7 +24225,7 @@
         <v>292</v>
       </c>
       <c r="B293" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C293" s="4" t="s">
         <v>27</v>
@@ -23972,7 +24308,7 @@
         <v>293</v>
       </c>
       <c r="B294" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C294" s="4" t="s">
         <v>27</v>
@@ -24046,7 +24382,7 @@
         <v>294</v>
       </c>
       <c r="B295" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C295" s="4" t="s">
         <v>27</v>
@@ -24120,7 +24456,7 @@
         <v>295</v>
       </c>
       <c r="B296" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C296" s="4" t="s">
         <v>27</v>
@@ -24200,7 +24536,7 @@
         <v>296</v>
       </c>
       <c r="B297" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C297" s="4" t="s">
         <v>27</v>
@@ -24283,7 +24619,7 @@
         <v>297</v>
       </c>
       <c r="B298" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C298" s="4" t="s">
         <v>27</v>
@@ -24357,7 +24693,7 @@
         <v>298</v>
       </c>
       <c r="B299" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C299" s="4" t="s">
         <v>27</v>
@@ -24437,7 +24773,7 @@
         <v>299</v>
       </c>
       <c r="B300" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C300" s="4" t="s">
         <v>27</v>
@@ -24517,7 +24853,7 @@
         <v>300</v>
       </c>
       <c r="B301" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C301" s="4" t="s">
         <v>27</v>
@@ -24600,7 +24936,7 @@
         <v>301</v>
       </c>
       <c r="B302" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C302" s="4" t="s">
         <v>27</v>
@@ -24680,7 +25016,7 @@
         <v>302</v>
       </c>
       <c r="B303" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C303" s="4" t="s">
         <v>27</v>
@@ -24763,7 +25099,7 @@
         <v>303</v>
       </c>
       <c r="B304" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C304" s="4" t="s">
         <v>27</v>
@@ -24843,7 +25179,7 @@
         <v>304</v>
       </c>
       <c r="B305" s="3">
-        <v>41966</v>
+        <v>41601</v>
       </c>
       <c r="C305" s="4" t="s">
         <v>27</v>
@@ -24926,7 +25262,7 @@
         <v>305</v>
       </c>
       <c r="B306" s="3">
-        <v>41970</v>
+        <v>41605</v>
       </c>
       <c r="C306" s="4" t="s">
         <v>85</v>
@@ -25009,7 +25345,7 @@
         <v>306</v>
       </c>
       <c r="B307" s="3">
-        <v>41970</v>
+        <v>41605</v>
       </c>
       <c r="C307" s="4" t="s">
         <v>85</v>
@@ -25092,7 +25428,7 @@
         <v>307</v>
       </c>
       <c r="B308" s="3">
-        <v>41970</v>
+        <v>41605</v>
       </c>
       <c r="C308" s="4" t="s">
         <v>85</v>
@@ -25175,7 +25511,7 @@
         <v>308</v>
       </c>
       <c r="B309" s="3">
-        <v>41970</v>
+        <v>41605</v>
       </c>
       <c r="C309" s="4" t="s">
         <v>85</v>
@@ -25255,7 +25591,7 @@
         <v>309</v>
       </c>
       <c r="B310" s="3">
-        <v>41970</v>
+        <v>41605</v>
       </c>
       <c r="C310" s="4" t="s">
         <v>85</v>
@@ -25329,7 +25665,7 @@
         <v>310</v>
       </c>
       <c r="B311" s="3">
-        <v>41970</v>
+        <v>41605</v>
       </c>
       <c r="C311" s="4" t="s">
         <v>85</v>
@@ -25409,7 +25745,7 @@
         <v>311</v>
       </c>
       <c r="B312" s="3">
-        <v>41970</v>
+        <v>41605</v>
       </c>
       <c r="C312" s="4" t="s">
         <v>85</v>
@@ -25489,7 +25825,7 @@
         <v>312</v>
       </c>
       <c r="B313" s="3">
-        <v>41977</v>
+        <v>41612</v>
       </c>
       <c r="C313" s="4" t="s">
         <v>85</v>
@@ -25572,7 +25908,7 @@
         <v>313</v>
       </c>
       <c r="B314" s="3">
-        <v>41977</v>
+        <v>41612</v>
       </c>
       <c r="C314" s="4" t="s">
         <v>85</v>
@@ -25652,7 +25988,7 @@
         <v>314</v>
       </c>
       <c r="B315" s="3">
-        <v>41977</v>
+        <v>41612</v>
       </c>
       <c r="C315" s="4" t="s">
         <v>85</v>
@@ -25735,7 +26071,7 @@
         <v>315</v>
       </c>
       <c r="B316" s="3">
-        <v>41977</v>
+        <v>41612</v>
       </c>
       <c r="C316" s="4" t="s">
         <v>85</v>
@@ -25815,7 +26151,7 @@
         <v>316</v>
       </c>
       <c r="B317" s="3">
-        <v>41977</v>
+        <v>41612</v>
       </c>
       <c r="C317" s="4" t="s">
         <v>85</v>
@@ -25895,7 +26231,7 @@
         <v>317</v>
       </c>
       <c r="B318" s="3">
-        <v>41977</v>
+        <v>41612</v>
       </c>
       <c r="C318" s="4" t="s">
         <v>85</v>
@@ -25969,7 +26305,7 @@
         <v>318</v>
       </c>
       <c r="B319" s="3">
-        <v>41977</v>
+        <v>41612</v>
       </c>
       <c r="C319" s="4" t="s">
         <v>85</v>
@@ -26052,7 +26388,7 @@
         <v>319</v>
       </c>
       <c r="B320" s="3">
-        <v>41977</v>
+        <v>41612</v>
       </c>
       <c r="C320" s="4" t="s">
         <v>85</v>
@@ -26126,7 +26462,7 @@
         <v>320</v>
       </c>
       <c r="B321" s="3">
-        <v>41977</v>
+        <v>41612</v>
       </c>
       <c r="C321" s="4" t="s">
         <v>85</v>
@@ -26206,7 +26542,7 @@
         <v>321</v>
       </c>
       <c r="B322" s="3">
-        <v>41977</v>
+        <v>41612</v>
       </c>
       <c r="C322" s="4" t="s">
         <v>85</v>
@@ -26286,7 +26622,7 @@
         <v>322</v>
       </c>
       <c r="B323" s="3">
-        <v>41986</v>
+        <v>41621</v>
       </c>
       <c r="C323" s="4" t="s">
         <v>76</v>
@@ -26360,7 +26696,7 @@
         <v>323</v>
       </c>
       <c r="B324" s="3">
-        <v>41986</v>
+        <v>41621</v>
       </c>
       <c r="C324" s="4" t="s">
         <v>76</v>
@@ -26434,7 +26770,7 @@
         <v>324</v>
       </c>
       <c r="B325" s="3">
-        <v>41986</v>
+        <v>41621</v>
       </c>
       <c r="C325" s="4" t="s">
         <v>76</v>
@@ -26508,7 +26844,7 @@
         <v>325</v>
       </c>
       <c r="B326" s="3">
-        <v>41986</v>
+        <v>41621</v>
       </c>
       <c r="C326" s="4" t="s">
         <v>76</v>
@@ -26582,7 +26918,7 @@
         <v>326</v>
       </c>
       <c r="B327" s="3">
-        <v>41986</v>
+        <v>41621</v>
       </c>
       <c r="C327" s="4" t="s">
         <v>76</v>
@@ -26656,7 +26992,7 @@
         <v>327</v>
       </c>
       <c r="B328" s="3">
-        <v>41987</v>
+        <v>41622</v>
       </c>
       <c r="C328" s="4" t="s">
         <v>85</v>
@@ -26730,7 +27066,7 @@
         <v>328</v>
       </c>
       <c r="B329" s="3">
-        <v>41987</v>
+        <v>41622</v>
       </c>
       <c r="C329" s="4" t="s">
         <v>85</v>
@@ -26810,7 +27146,7 @@
         <v>329</v>
       </c>
       <c r="B330" s="3">
-        <v>41987</v>
+        <v>41622</v>
       </c>
       <c r="C330" s="4" t="s">
         <v>85</v>
@@ -26890,7 +27226,7 @@
         <v>330</v>
       </c>
       <c r="B331" s="3">
-        <v>41987</v>
+        <v>41622</v>
       </c>
       <c r="C331" s="4" t="s">
         <v>85</v>
@@ -26970,7 +27306,7 @@
         <v>331</v>
       </c>
       <c r="B332" s="3">
-        <v>41987</v>
+        <v>41622</v>
       </c>
       <c r="C332" s="4" t="s">
         <v>90</v>
@@ -27050,7 +27386,7 @@
         <v>332</v>
       </c>
       <c r="B333" s="3">
-        <v>41987</v>
+        <v>41622</v>
       </c>
       <c r="C333" s="4" t="s">
         <v>90</v>
@@ -27130,7 +27466,7 @@
         <v>333</v>
       </c>
       <c r="B334" s="3">
-        <v>41987</v>
+        <v>41622</v>
       </c>
       <c r="C334" s="4" t="s">
         <v>90</v>
@@ -27213,7 +27549,7 @@
         <v>334</v>
       </c>
       <c r="B335" s="3">
-        <v>41987</v>
+        <v>41622</v>
       </c>
       <c r="C335" s="4" t="s">
         <v>90</v>
@@ -27287,7 +27623,7 @@
         <v>335</v>
       </c>
       <c r="B336" s="3">
-        <v>41987</v>
+        <v>41622</v>
       </c>
       <c r="C336" s="4" t="s">
         <v>90</v>
@@ -27370,7 +27706,7 @@
         <v>336</v>
       </c>
       <c r="B337" s="3">
-        <v>41987</v>
+        <v>41622</v>
       </c>
       <c r="C337" s="4" t="s">
         <v>90</v>
@@ -27453,7 +27789,7 @@
         <v>337</v>
       </c>
       <c r="B338" s="3">
-        <v>41987</v>
+        <v>41622</v>
       </c>
       <c r="C338" s="4" t="s">
         <v>90</v>
@@ -27527,7 +27863,7 @@
         <v>338</v>
       </c>
       <c r="B339" s="3">
-        <v>41987</v>
+        <v>41622</v>
       </c>
       <c r="C339" s="4" t="s">
         <v>90</v>
@@ -27610,7 +27946,7 @@
         <v>339</v>
       </c>
       <c r="B340" s="3">
-        <v>41987</v>
+        <v>41622</v>
       </c>
       <c r="C340" s="4" t="s">
         <v>90</v>
@@ -27684,7 +28020,7 @@
         <v>340</v>
       </c>
       <c r="B341" s="3">
-        <v>41987</v>
+        <v>41622</v>
       </c>
       <c r="C341" s="4" t="s">
         <v>90</v>
@@ -27764,7 +28100,7 @@
         <v>341</v>
       </c>
       <c r="B342" s="3">
-        <v>41987</v>
+        <v>41622</v>
       </c>
       <c r="C342" s="4" t="s">
         <v>90</v>
@@ -27838,7 +28174,7 @@
         <v>342</v>
       </c>
       <c r="B343" s="3">
-        <v>41987</v>
+        <v>41622</v>
       </c>
       <c r="C343" s="4" t="s">
         <v>90</v>
@@ -27921,7 +28257,7 @@
         <v>343</v>
       </c>
       <c r="B344" s="3">
-        <v>41987</v>
+        <v>41622</v>
       </c>
       <c r="C344" s="4" t="s">
         <v>90</v>
@@ -27995,7 +28331,7 @@
         <v>344</v>
       </c>
       <c r="B345" s="3">
-        <v>41987</v>
+        <v>41622</v>
       </c>
       <c r="C345" s="4" t="s">
         <v>90</v>
@@ -28069,7 +28405,7 @@
         <v>345</v>
       </c>
       <c r="B346" s="3">
-        <v>41987</v>
+        <v>41622</v>
       </c>
       <c r="C346" s="4" t="s">
         <v>90</v>
@@ -28149,7 +28485,7 @@
         <v>346</v>
       </c>
       <c r="B347" s="3">
-        <v>41987</v>
+        <v>41622</v>
       </c>
       <c r="C347" s="4" t="s">
         <v>90</v>

</xml_diff>